<commit_message>
Updated calculations and summary statistics
Removed calculations not included in revised manuscript
</commit_message>
<xml_diff>
--- a/iTTC/statistics table.xlsx
+++ b/iTTC/statistics table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TAMU\Weihsueh lab\TTC\iTTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wchiu/Dropbox/WCHIU-Documents/TK_TeA/iTTC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37E62D5-519C-480B-8AD7-1805AC5E2355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D95881-C196-1944-8D91-A2001DF6DE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22450" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{354831FC-B8F7-48ED-9F71-B6963CDC090B}"/>
+    <workbookView xWindow="-740" yWindow="-20420" windowWidth="33600" windowHeight="18940" xr2:uid="{354831FC-B8F7-48ED-9F71-B6963CDC090B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Truong</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,6 +105,12 @@
   <si>
     <t>control</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>95th</t>
   </si>
 </sst>
 </file>
@@ -126,14 +121,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -506,36 +501,36 @@
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.09765625" customWidth="1"/>
-    <col min="6" max="6" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.09765625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.09765625" customWidth="1"/>
-    <col min="16" max="16" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.09765625" customWidth="1"/>
-    <col min="21" max="21" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.8984375" customWidth="1"/>
-    <col min="26" max="26" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1640625" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1640625" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.83203125" customWidth="1"/>
+    <col min="26" max="26" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -552,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -623,13 +618,13 @@
         <v>17</v>
       </c>
       <c r="Z2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="AA2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -697,22 +692,22 @@
         <v>34.281337753142601</v>
       </c>
       <c r="W3" s="1">
-        <v>9.35</v>
+        <v>3.64</v>
       </c>
       <c r="X3" s="1">
-        <v>2.91</v>
+        <v>0.04</v>
       </c>
       <c r="Y3" s="1">
-        <v>24.42</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="Z3" s="1">
-        <v>1.61</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="1">
-        <v>39.81</v>
+        <v>46.64</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -780,22 +775,22 @@
         <v>122.922020186431</v>
       </c>
       <c r="W4" s="1">
-        <v>2.395</v>
+        <v>1.59</v>
       </c>
       <c r="X4" s="1">
-        <v>1.4475</v>
+        <v>0.6</v>
       </c>
       <c r="Y4" s="1">
-        <v>6.51</v>
+        <v>5.39</v>
       </c>
       <c r="Z4" s="1">
-        <v>0.56999999999999995</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="1">
-        <v>78.2</v>
+        <v>22.15</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -863,22 +858,22 @@
         <v>10.039003463501601</v>
       </c>
       <c r="W5" s="1">
-        <v>1.94</v>
+        <v>0</v>
       </c>
       <c r="X5" s="1">
-        <v>1.39</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>4.3099999999999996</v>
+        <v>0.66</v>
       </c>
       <c r="Z5" s="1">
         <v>0</v>
       </c>
       <c r="AA5" s="1">
-        <v>11.07</v>
+        <v>12.48</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -958,10 +953,10 @@
         <v>0</v>
       </c>
       <c r="AA6" s="1">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1041,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="AA7" s="2">
-        <v>0.19</v>
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>